<commit_message>
fixed french excel file
</commit_message>
<xml_diff>
--- a/bulk-upload-templates/fr/FR_E-Label_Template.xlsx
+++ b/bulk-upload-templates/fr/FR_E-Label_Template.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maxbauer/workspace/vs_code/misc/e-label.io/bulk-upload-templates/fr/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E2E5808-1ABC-B443-A584-F4526C1FB712}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3417CCE1-EAFC-404E-8B30-6887E96E9517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17960" activeTab="1" xr2:uid="{42B7CF4C-2976-4744-81A6-4766AD4B0A9A}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17960" xr2:uid="{42B7CF4C-2976-4744-81A6-4766AD4B0A9A}"/>
   </bookViews>
   <sheets>
-    <sheet name="E-Label Upload" sheetId="1" state="hidden" r:id="rId1"/>
-    <sheet name="Erlaubte Zutaten" sheetId="2" r:id="rId2"/>
+    <sheet name="E-Label Upload" sheetId="1" r:id="rId1"/>
+    <sheet name="Erlaubte Zutaten" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -770,9 +770,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4271114-3DDD-3644-B3E5-81C7199578E4}">
   <dimension ref="A1:O1147"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J1" sqref="J1:J1048576"/>
+      <selection pane="bottomLeft" activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -850,7 +850,7 @@
         <v>4</v>
       </c>
       <c r="D2" s="32">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="E2" s="32">
         <v>750</v>
@@ -18844,7 +18844,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFB2A205-F100-5742-AB12-7F9C1E480E50}">
   <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>

</xml_diff>